<commit_message>
Update website design and features
</commit_message>
<xml_diff>
--- a/employee_projects.xlsx
+++ b/employee_projects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a0432cb4d8ab5c17/Desktop/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{1487A758-DAE2-4A5F-BF3B-028E260786D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5752A461-F04A-43E8-8537-78FCCB47F3AD}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{1487A758-DAE2-4A5F-BF3B-028E260786D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A572EBD-5932-45E3-9F17-0E9795B81D99}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FE1FB76F-4A36-46E4-922B-87998CCDF517}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Salem</t>
-  </si>
-  <si>
-    <t>Alpha</t>
-  </si>
-  <si>
-    <t>Beta</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -68,15 +59,9 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Theta</t>
-  </si>
-  <si>
     <t>Mohammed</t>
   </si>
   <si>
-    <t>Malik</t>
-  </si>
-  <si>
     <t>Finance</t>
   </si>
   <si>
@@ -86,31 +71,76 @@
     <t>WFD</t>
   </si>
   <si>
-    <t>$900</t>
-  </si>
-  <si>
-    <t>$901</t>
-  </si>
-  <si>
-    <t>$902</t>
-  </si>
-  <si>
-    <t>$903</t>
-  </si>
-  <si>
-    <t>$904</t>
-  </si>
-  <si>
-    <t>$905</t>
-  </si>
-  <si>
-    <t>$906</t>
-  </si>
-  <si>
-    <t>Sarah</t>
-  </si>
-  <si>
-    <t>Ali</t>
+    <t>Smart Factory</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>AI OPT.</t>
+  </si>
+  <si>
+    <t>Talent</t>
+  </si>
+  <si>
+    <t>Sustainability</t>
+  </si>
+  <si>
+    <t>Muruj Allhiby</t>
+  </si>
+  <si>
+    <t>Leen Khalid</t>
+  </si>
+  <si>
+    <t>Ali Alharbi</t>
+  </si>
+  <si>
+    <t>Sarah Almutairi</t>
+  </si>
+  <si>
+    <t>Salem Ali</t>
+  </si>
+  <si>
+    <t>Malik M.</t>
+  </si>
+  <si>
+    <t>Yussef Y.</t>
+  </si>
+  <si>
+    <t>$9000</t>
+  </si>
+  <si>
+    <t>$9001</t>
+  </si>
+  <si>
+    <t>$9002</t>
+  </si>
+  <si>
+    <t>$9003</t>
+  </si>
+  <si>
+    <t>$9004</t>
+  </si>
+  <si>
+    <t>$9005</t>
+  </si>
+  <si>
+    <t>$9006</t>
+  </si>
+  <si>
+    <t>$9007</t>
+  </si>
+  <si>
+    <t>$9008</t>
+  </si>
+  <si>
+    <t>$9009</t>
+  </si>
+  <si>
+    <t>$9010</t>
+  </si>
+  <si>
+    <t>$9011</t>
   </si>
 </sst>
 </file>
@@ -492,27 +522,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76548872-9A0E-4750-95C8-2757DC80BC8A}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.90625" customWidth="1"/>
     <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
     <col min="4" max="4" width="12.6328125" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -521,150 +551,250 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1234</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1122</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1235</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>1111</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>1111</v>
       </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>1111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>1111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="D8">
+      <c r="B11">
+        <v>1111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>1111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>